<commit_message>
Changes 2 to 17
</commit_message>
<xml_diff>
--- a/GitTest_01.xlsx
+++ b/GitTest_01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22104" windowHeight="11244"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="22104" windowHeight="11244"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -394,7 +394,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -419,7 +419,7 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>SUM(A2:A5)</f>
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>